<commit_message>
Mo ta chuc nang v1
</commit_message>
<xml_diff>
--- a/Analysis/Plant/BKProject_Motachucnang.xlsx
+++ b/Analysis/Plant/BKProject_Motachucnang.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>STT</t>
   </si>
@@ -34,15 +34,6 @@
     <t>Tim kiếm</t>
   </si>
   <si>
-    <t>Có thể tìm kiếm theo bài viết, thành viên,…</t>
-  </si>
-  <si>
-    <t>Post, comment</t>
-  </si>
-  <si>
-    <t>Comment bằng face</t>
-  </si>
-  <si>
     <t>Vinh danh</t>
   </si>
   <si>
@@ -50,13 +41,100 @@
   </si>
   <si>
     <t>Các chức năng của hệ thống BK Project</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Đang xem xét</t>
+  </si>
+  <si>
+    <t>Trạng thái</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Các tính năng ở trạng thái đang xem xét khi chuyển thành ok hoặc hủy sẽ ở dạng Đang xem xét | OK </t>
+  </si>
+  <si>
+    <t>hoặc Đang xem xét |Hủy</t>
+  </si>
+  <si>
+    <t>Độ ưu tiên</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Đăng kí tìm nhà theo yêu cầu </t>
+  </si>
+  <si>
+    <t>Cho phép người dùng tìm kiếm nhà theo yêu cầu ( diện tích, khoảng tiền, địa điểm, số người, chung chủ, ko chung chủ ,…</t>
+  </si>
+  <si>
+    <t>Thông báo khi phát hiện bản tin đăng cho thuê nhà</t>
+  </si>
+  <si>
+    <t>Thông báo cho những người đăng kí tìm nhà đã có nhà thỏa mãn</t>
+  </si>
+  <si>
+    <t>Post, comment, xóa bài</t>
+  </si>
+  <si>
+    <t>Cho phép post bài, comment, xóa bài đã post hoặc comment</t>
+  </si>
+  <si>
+    <t>Lưu tin</t>
+  </si>
+  <si>
+    <t>Cho phép lưu bản tin đã xem</t>
+  </si>
+  <si>
+    <t>Có thể tìm kiếm theo bài viết, thành viên, tìm kiếm theo các lựa chọn (tiền, địa điểm, diện tích,…)</t>
+  </si>
+  <si>
+    <t>Sắp xếp</t>
+  </si>
+  <si>
+    <t>Cho phép người dùng sắp xếp các bản tin theo loại tin (cho thuê, tìm nhà thuê, thuê nguyên căn,..), giá, địa điểm, diện tích, đối tượng ( nam, nữ)</t>
+  </si>
+  <si>
+    <t>Gợi ý</t>
+  </si>
+  <si>
+    <t>Dựa vào các dữ liệu cuar những phiên giao dịch trước, dự đoán xem các đối tượng sẽ thuê phòng ở chỗ nào, sau đó gợi ý cho người dùng về ( các khu vực nhà giá rẻ, khu vực diện tích rộng, khu vực gần xe bus, khu vực đông, ít dân cư, gần chợ,…). Tuy nhiên đang có vẻ trùng với tìm kiếm ( giải pháp có thể là xây dựng tìm kiếm thông minh kiêm gợi ý)</t>
+  </si>
+  <si>
+    <t>Bộ lọc</t>
+  </si>
+  <si>
+    <t>Lọc những tin rác, tin của cò mồi</t>
+  </si>
+  <si>
+    <t>Đánh dấu spam, đánh dấu black list</t>
+  </si>
+  <si>
+    <t>Cho phép người dùng có thể đánh dấu 1 tin là của cò mồi, spam, hoặc lừa đảo ( khi đã đánh dấu, thành viên đó sẽ bị nâng mã bảo mật lên cấp 2, nếu bị đánh dấu nhiều, block nick, bôi đen nick, (vẫn giữ lại toàn bộ bài viết) và đưa vào mục black list</t>
+  </si>
+  <si>
+    <t>Black list</t>
+  </si>
+  <si>
+    <t>Danh sách nick bị block do lừa đảo, ko uy tín</t>
+  </si>
+  <si>
+    <t>Nap tiền duy trì tin</t>
+  </si>
+  <si>
+    <t>Khi ở trạng thái free, bản tin có thể được thông báo đến các đối tượng cần tìm nhà trong khoảng x ngày, nếu nạp tiền thì sẽ tăng khoảng thời gian, đồng thời tin đó được hiển thị nhiều hơn trên trang chủ, hoặc ưu tiên khi tìm kiếm</t>
+  </si>
+  <si>
+    <t>Gop ý</t>
+  </si>
+  <si>
+    <t>Người dùng có thể góp ý với admin về hệ thống</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,13 +142,52 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="163"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="163"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="163"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -137,28 +254,80 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,214 +632,285 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="10" width="8.88671875" style="1"/>
+    <col min="11" max="11" width="28.5546875" style="1" customWidth="1"/>
+    <col min="12" max="13" width="8.88671875" style="1"/>
+    <col min="14" max="14" width="7.88671875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="8.77734375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="15.44140625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="11.6640625" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.88671875" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="H1" s="10" t="s">
+    <row r="1" spans="1:17" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="H1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="Q5" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="18">
         <v>1</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="3" t="s">
+      <c r="B6" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q6" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="18">
         <v>2</v>
       </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="5"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+      <c r="B7" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q7" s="28">
         <v>1</v>
       </c>
-      <c r="B5" s="2" t="s">
+    </row>
+    <row r="8" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="18">
         <v>3</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="7" t="s">
+      <c r="B8" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="22"/>
+      <c r="P8" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q8" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="18">
         <v>4</v>
       </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="9"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>2</v>
-      </c>
-      <c r="B6" s="6" t="s">
+      <c r="B9" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q9" s="17"/>
+    </row>
+    <row r="10" spans="1:17" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10">
         <v>5</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="7" t="s">
+      <c r="B10" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
+      <c r="K10" s="26"/>
+      <c r="L10" s="26"/>
+      <c r="M10" s="26"/>
+      <c r="N10" s="26"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="10">
         <v>6</v>
       </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="9"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>3</v>
-      </c>
-      <c r="B7" s="6" t="s">
+      <c r="B11" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="26"/>
+      <c r="N11" s="26"/>
+      <c r="O11" s="27"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="10">
         <v>7</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="7" t="s">
+      <c r="B12" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="26"/>
+      <c r="O12" s="27"/>
+      <c r="P12" s="17"/>
+      <c r="Q12" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="28.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
         <v>8</v>
       </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="9"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>4</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="9"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="9"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="9"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="9"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="9"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="6"/>
+      <c r="B13" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
-      <c r="H13" s="7"/>
+      <c r="H13" s="7" t="s">
+        <v>25</v>
+      </c>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
@@ -678,16 +918,26 @@
       <c r="M13" s="8"/>
       <c r="N13" s="8"/>
       <c r="O13" s="9"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="6"/>
+      <c r="P13" s="5"/>
+      <c r="Q13" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <v>9</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
-      <c r="H14" s="7"/>
+      <c r="H14" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
@@ -695,16 +945,26 @@
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
       <c r="O14" s="9"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="6"/>
+      <c r="P14" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q14" s="5"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>10</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="7"/>
+      <c r="H15" s="7" t="s">
+        <v>29</v>
+      </c>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
@@ -712,16 +972,26 @@
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
       <c r="O15" s="9"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="6"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="47.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>11</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="7"/>
+      <c r="H16" s="7" t="s">
+        <v>31</v>
+      </c>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
@@ -729,16 +999,26 @@
       <c r="M16" s="8"/>
       <c r="N16" s="8"/>
       <c r="O16" s="9"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="B17" s="6"/>
+      <c r="P16" s="5"/>
+      <c r="Q16" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>12</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
-      <c r="H17" s="7"/>
+      <c r="H17" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
@@ -746,16 +1026,26 @@
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
       <c r="O17" s="9"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="B18" s="6"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>13</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
-      <c r="H18" s="7"/>
+      <c r="H18" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
@@ -763,19 +1053,54 @@
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>
       <c r="O18" s="9"/>
+      <c r="P18" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q18" s="5"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>14</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="H1:K1"/>
-    <mergeCell ref="H13:O13"/>
-    <mergeCell ref="H14:O14"/>
-    <mergeCell ref="H15:O15"/>
-    <mergeCell ref="H16:O16"/>
-    <mergeCell ref="H17:O17"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="H5:O5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B11:G11"/>
     <mergeCell ref="H18:O18"/>
-    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="H19:O19"/>
     <mergeCell ref="B18:G18"/>
-    <mergeCell ref="H5:O5"/>
+    <mergeCell ref="B19:G19"/>
     <mergeCell ref="H6:O6"/>
     <mergeCell ref="H7:O7"/>
     <mergeCell ref="H8:O8"/>
@@ -783,21 +1108,18 @@
     <mergeCell ref="H10:O10"/>
     <mergeCell ref="H11:O11"/>
     <mergeCell ref="H12:O12"/>
-    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="H13:O13"/>
     <mergeCell ref="B12:G12"/>
     <mergeCell ref="B13:G13"/>
     <mergeCell ref="B14:G14"/>
     <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="H4:O4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="H14:O14"/>
+    <mergeCell ref="H15:O15"/>
+    <mergeCell ref="H16:O16"/>
+    <mergeCell ref="H17:O17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>